<commit_message>
- changed theme colors and fixed DataTableEditTextField - added remove action for rows in single-selection data table - added IFilePicker
- need to implement actual importing measurements from JSON/EXCEL
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -12,33 +12,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
-    <t>ID</t>
+    <t>Идентификатор</t>
   </si>
   <si>
     <t>Описание</t>
   </si>
   <si>
-    <t>Комментарий</t>
+    <t>Единица измерения</t>
   </si>
   <si>
-    <t>Партия</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>тест1</t>
-  </si>
-  <si>
-    <t>тест2</t>
+    <t>icc3</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>2</t>
+    <t>icc</t>
+  </si>
+  <si>
+    <t>icc1</t>
+  </si>
+  <si>
+    <t>А</t>
+  </si>
+  <si>
+    <t>icc4</t>
+  </si>
+  <si>
+    <t>icc2</t>
   </si>
 </sst>
 </file>
@@ -83,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -99,35 +102,59 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
+      <c r="B5" t="s">
+        <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
+      <c r="C5" t="s">
+        <v>4</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>